<commit_message>
Added link to acceptance test plan excel sheet
</commit_message>
<xml_diff>
--- a/etc/Acceptance Test Plan.xlsx
+++ b/etc/Acceptance Test Plan.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="108">
   <si>
     <t>Instructions</t>
   </si>
@@ -205,6 +205,9 @@
   </si>
   <si>
     <t>User Login Page</t>
+  </si>
+  <si>
+    <t>As a user of the website I want to be able to login so that I can use the website.</t>
   </si>
   <si>
     <t>Given I am a customer when I want to login to the website then I expect to be able to login at a login page</t>
@@ -4692,15 +4695,17 @@
       <c r="Z27" s="12"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="2"/>
+      <c r="A28" s="10" t="s">
+        <v>61</v>
+      </c>
       <c r="B28" s="10" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>13</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E28" s="11"/>
       <c r="F28" s="2"/>
@@ -4728,13 +4733,13 @@
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="2"/>
       <c r="B29" s="10" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>13</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E29" s="11"/>
       <c r="F29" s="2"/>
@@ -4761,7 +4766,7 @@
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="19" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B30" s="19"/>
       <c r="C30" s="11"/>
@@ -4791,16 +4796,16 @@
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>13</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E31" s="11"/>
       <c r="F31" s="2"/>
@@ -4828,13 +4833,13 @@
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="10"/>
       <c r="B32" s="10" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>13</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E32" s="11"/>
       <c r="F32" s="2"/>
@@ -4861,7 +4866,7 @@
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="19" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B33" s="20"/>
       <c r="C33" s="11"/>
@@ -4891,16 +4896,16 @@
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="10" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>13</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E34" s="11"/>
       <c r="F34" s="2"/>
@@ -4928,13 +4933,13 @@
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="2"/>
       <c r="B35" s="10" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C35" s="9" t="s">
         <v>13</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E35" s="11"/>
       <c r="F35" s="2"/>
@@ -4961,7 +4966,7 @@
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="19" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B36" s="20"/>
       <c r="C36" s="11"/>
@@ -4991,16 +4996,16 @@
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="10" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C37" s="9" t="s">
         <v>13</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E37" s="11"/>
       <c r="F37" s="2"/>
@@ -5028,13 +5033,13 @@
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="2"/>
       <c r="B38" s="10" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C38" s="9" t="s">
         <v>13</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E38" s="11"/>
       <c r="F38" s="2"/>
@@ -5061,7 +5066,7 @@
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="19" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B39" s="20"/>
       <c r="C39" s="11"/>
@@ -5091,16 +5096,16 @@
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="10" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C40" s="9" t="s">
         <v>13</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E40" s="11"/>
       <c r="F40" s="2"/>
@@ -5128,13 +5133,13 @@
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="2"/>
       <c r="B41" s="10" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C41" s="9" t="s">
         <v>13</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E41" s="11"/>
       <c r="F41" s="2"/>
@@ -5161,7 +5166,7 @@
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="19" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B42" s="20"/>
       <c r="C42" s="11"/>
@@ -5191,16 +5196,16 @@
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="10" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C43" s="9" t="s">
         <v>13</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E43" s="11"/>
       <c r="F43" s="2"/>
@@ -5228,13 +5233,13 @@
     <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="2"/>
       <c r="B44" s="10" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C44" s="9" t="s">
         <v>13</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E44" s="11"/>
       <c r="F44" s="2"/>
@@ -5261,7 +5266,7 @@
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="19" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B45" s="20"/>
       <c r="C45" s="11"/>
@@ -5291,16 +5296,16 @@
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="10" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C46" s="9" t="s">
         <v>13</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E46" s="11"/>
       <c r="F46" s="2"/>
@@ -5328,13 +5333,13 @@
     <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="2"/>
       <c r="B47" s="10" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C47" s="9" t="s">
         <v>13</v>
       </c>
       <c r="D47" s="10" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E47" s="11"/>
       <c r="F47" s="2"/>
@@ -5361,7 +5366,7 @@
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="19" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B48" s="20"/>
       <c r="C48" s="11"/>
@@ -5391,16 +5396,16 @@
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="10" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C49" s="9" t="s">
         <v>13</v>
       </c>
       <c r="D49" s="10" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E49" s="11"/>
       <c r="F49" s="2"/>
@@ -5428,13 +5433,13 @@
     <row r="50" ht="15.75" customHeight="1">
       <c r="A50" s="2"/>
       <c r="B50" s="10" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C50" s="9" t="s">
         <v>13</v>
       </c>
       <c r="D50" s="10" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E50" s="11"/>
       <c r="F50" s="2"/>

</xml_diff>